<commit_message>
Switch in designlabels switched to numeric
</commit_message>
<xml_diff>
--- a/data/Arduino_trainingset_3VarsDesign.xlsx
+++ b/data/Arduino_trainingset_3VarsDesign.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="10">
   <si>
     <t>F1</t>
   </si>
@@ -41,13 +41,7 @@
     <t>F4</t>
   </si>
   <si>
-    <t>power_off</t>
-  </si>
-  <si>
     <t>?</t>
-  </si>
-  <si>
-    <t>power_on</t>
   </si>
   <si>
     <t>F</t>
@@ -425,7 +419,7 @@
   <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -436,13 +430,13 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>9</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>11</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>0</v>
@@ -461,8 +455,8 @@
       <c r="A2" s="4">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
-        <v>6</v>
+      <c r="B2">
+        <v>1</v>
       </c>
       <c r="C2">
         <v>1.8</v>
@@ -471,24 +465,24 @@
         <v>1.8</v>
       </c>
       <c r="E2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="4">
         <v>1</v>
       </c>
-      <c r="B3" t="s">
-        <v>6</v>
+      <c r="B3">
+        <v>1</v>
       </c>
       <c r="C3">
         <v>0.5</v>
@@ -497,24 +491,24 @@
         <v>0</v>
       </c>
       <c r="E3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="H3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="4">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
-        <v>6</v>
+      <c r="B4">
+        <v>1</v>
       </c>
       <c r="C4">
         <v>0</v>
@@ -523,24 +517,24 @@
         <v>0</v>
       </c>
       <c r="E4" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F4" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="G4" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="H4" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="4">
         <v>4</v>
       </c>
-      <c r="B5" t="s">
-        <v>6</v>
+      <c r="B5">
+        <v>1</v>
       </c>
       <c r="C5">
         <v>2.1</v>
@@ -549,24 +543,24 @@
         <v>1.8</v>
       </c>
       <c r="E5" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F5" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="G5" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="H5" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="4">
         <v>5</v>
       </c>
-      <c r="B6" t="s">
-        <v>6</v>
+      <c r="B6">
+        <v>1</v>
       </c>
       <c r="C6">
         <v>0.6</v>
@@ -575,24 +569,24 @@
         <v>0</v>
       </c>
       <c r="E6" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F6" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="G6" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="H6" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="4">
         <v>6</v>
       </c>
-      <c r="B7" t="s">
-        <v>6</v>
+      <c r="B7">
+        <v>1</v>
       </c>
       <c r="C7">
         <v>5</v>
@@ -601,24 +595,24 @@
         <v>4.5999999999999996</v>
       </c>
       <c r="E7" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="F7" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G7" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="H7" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="4">
         <v>7</v>
       </c>
-      <c r="B8" t="s">
-        <v>6</v>
+      <c r="B8">
+        <v>1</v>
       </c>
       <c r="C8">
         <v>5</v>
@@ -627,24 +621,24 @@
         <v>0</v>
       </c>
       <c r="E8" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="F8" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G8" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="H8" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="4">
         <v>8</v>
       </c>
-      <c r="B9" t="s">
-        <v>6</v>
+      <c r="B9">
+        <v>1</v>
       </c>
       <c r="C9">
         <v>5</v>
@@ -653,24 +647,24 @@
         <v>5</v>
       </c>
       <c r="E9" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="F9" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="G9" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="H9" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="4">
         <v>9</v>
       </c>
-      <c r="B10" t="s">
-        <v>6</v>
+      <c r="B10">
+        <v>1</v>
       </c>
       <c r="C10">
         <v>2.4</v>
@@ -679,24 +673,24 @@
         <v>2.4</v>
       </c>
       <c r="E10" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="F10" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="G10" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="H10" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="4">
         <v>10</v>
       </c>
-      <c r="B11" t="s">
-        <v>6</v>
+      <c r="B11">
+        <v>1</v>
       </c>
       <c r="C11">
         <v>5</v>
@@ -705,24 +699,24 @@
         <v>4.4000000000000004</v>
       </c>
       <c r="E11" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="F11" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="G11" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="H11" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="4">
         <v>11</v>
       </c>
-      <c r="B12" t="s">
-        <v>6</v>
+      <c r="B12">
+        <v>1</v>
       </c>
       <c r="C12">
         <v>3.4</v>
@@ -731,24 +725,24 @@
         <v>1.4</v>
       </c>
       <c r="E12" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="F12" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="G12" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="H12" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="4">
         <v>12</v>
       </c>
-      <c r="B13" t="s">
-        <v>4</v>
+      <c r="B13">
+        <v>0</v>
       </c>
       <c r="C13">
         <v>1.8</v>
@@ -757,50 +751,50 @@
         <v>1.8</v>
       </c>
       <c r="E13" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F13" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G13" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H13" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" s="4">
         <v>13</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14">
+        <v>0</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+      <c r="E14" t="s">
         <v>4</v>
       </c>
-      <c r="C14">
-        <v>0</v>
-      </c>
-      <c r="D14">
-        <v>0</v>
-      </c>
-      <c r="E14" t="s">
-        <v>5</v>
-      </c>
       <c r="F14" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G14" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H14" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" s="4">
         <v>16</v>
       </c>
-      <c r="B15" t="s">
-        <v>4</v>
+      <c r="B15">
+        <v>0</v>
       </c>
       <c r="C15">
         <v>2.1</v>
@@ -809,24 +803,24 @@
         <v>1.8</v>
       </c>
       <c r="E15" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F15" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="G15" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="H15" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" s="4">
         <v>17</v>
       </c>
-      <c r="B16" t="s">
-        <v>4</v>
+      <c r="B16">
+        <v>0</v>
       </c>
       <c r="C16">
         <v>0.7</v>
@@ -835,24 +829,24 @@
         <v>0</v>
       </c>
       <c r="E16" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F16" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="G16" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="H16" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" s="4">
         <v>18</v>
       </c>
-      <c r="B17" t="s">
-        <v>4</v>
+      <c r="B17">
+        <v>0</v>
       </c>
       <c r="C17">
         <v>0</v>
@@ -861,16 +855,16 @@
         <v>0.5</v>
       </c>
       <c r="E17" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="F17" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G17" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="H17" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>